<commit_message>
Fix missing type declarations on some IndexTable variables
</commit_message>
<xml_diff>
--- a/dds/installation.xlsx
+++ b/dds/installation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\dds\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="585" yWindow="1005" windowWidth="16380" windowHeight="7170" tabRatio="804"/>
+    <workbookView xWindow="590" yWindow="1010" windowWidth="16380" windowHeight="7170" tabRatio="804" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="1143">
   <si>
     <t>Identifier</t>
   </si>
@@ -3457,8 +3462,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3781,6 +3786,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3828,7 +3836,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3863,7 +3871,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4077,30 +4085,30 @@
   </sheetPr>
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="53.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="64.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="175.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="64.54296875" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="175.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="20.140625" style="18"/>
-    <col min="1027" max="16384" width="9.140625" style="18"/>
+    <col min="13" max="13" width="24.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="20.1796875" style="18"/>
+    <col min="1027" max="16384" width="9.1796875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="15" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="17" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>219</v>
       </c>
@@ -4164,7 +4172,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="17" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>220</v>
       </c>
@@ -4187,7 +4195,7 @@
       <c r="L3" s="16"/>
       <c r="M3" s="25"/>
     </row>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="17" customFormat="1">
       <c r="A4" s="9" t="s">
         <v>383</v>
       </c>
@@ -4210,7 +4218,7 @@
       <c r="L4" s="16"/>
       <c r="M4" s="25"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="17" customFormat="1">
       <c r="A5" s="9" t="s">
         <v>221</v>
       </c>
@@ -4233,7 +4241,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="25"/>
     </row>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="17" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>386</v>
       </c>
@@ -4256,7 +4264,7 @@
       <c r="L6" s="16"/>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="17" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>384</v>
       </c>
@@ -4279,7 +4287,7 @@
       <c r="L7" s="16"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="17" customFormat="1">
       <c r="A8" s="11" t="s">
         <v>385</v>
       </c>
@@ -4302,7 +4310,7 @@
       <c r="L8" s="16"/>
       <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="17" customFormat="1">
       <c r="A9" s="9" t="s">
         <v>222</v>
       </c>
@@ -4325,7 +4333,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="25"/>
     </row>
-    <row r="10" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="17" customFormat="1">
       <c r="A10" s="9" t="s">
         <v>223</v>
       </c>
@@ -4348,7 +4356,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="25"/>
     </row>
-    <row r="11" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="17" customFormat="1">
       <c r="A11" s="9" t="s">
         <v>224</v>
       </c>
@@ -4371,7 +4379,7 @@
       <c r="L11" s="16"/>
       <c r="M11" s="25"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="22" t="s">
         <v>226</v>
       </c>
@@ -4387,7 +4395,7 @@
       </c>
       <c r="M12" s="25"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="22" t="s">
         <v>225</v>
       </c>
@@ -4403,7 +4411,7 @@
       </c>
       <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="30" t="s">
         <v>863</v>
       </c>
@@ -4417,7 +4425,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="30" t="s">
         <v>339</v>
       </c>
@@ -4432,7 +4440,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="30" t="s">
         <v>351</v>
       </c>
@@ -4447,7 +4455,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="30" t="s">
         <v>846</v>
       </c>
@@ -4461,7 +4469,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="30" t="s">
         <v>847</v>
       </c>
@@ -4475,7 +4483,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="30" t="s">
         <v>848</v>
       </c>
@@ -4489,7 +4497,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="30" t="s">
         <v>849</v>
       </c>
@@ -4503,7 +4511,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="30" t="s">
         <v>850</v>
       </c>
@@ -4517,7 +4525,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="30" t="s">
         <v>851</v>
       </c>
@@ -4531,7 +4539,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="30" t="s">
         <v>352</v>
       </c>
@@ -4546,7 +4554,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="30" t="s">
         <v>375</v>
       </c>
@@ -4561,7 +4569,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="30" t="s">
         <v>340</v>
       </c>
@@ -4576,7 +4584,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="30" t="s">
         <v>342</v>
       </c>
@@ -4591,7 +4599,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="30" t="s">
         <v>343</v>
       </c>
@@ -4606,7 +4614,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="30" t="s">
         <v>344</v>
       </c>
@@ -4621,7 +4629,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="30" t="s">
         <v>345</v>
       </c>
@@ -4636,7 +4644,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="30" t="s">
         <v>943</v>
       </c>
@@ -4651,7 +4659,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="30" t="s">
         <v>942</v>
       </c>
@@ -4666,7 +4674,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="30" t="s">
         <v>557</v>
       </c>
@@ -4680,7 +4688,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="30" t="s">
         <v>558</v>
       </c>
@@ -4694,7 +4702,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="30" t="s">
         <v>559</v>
       </c>
@@ -4708,7 +4716,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="30" t="s">
         <v>562</v>
       </c>
@@ -4722,7 +4730,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="30" t="s">
         <v>560</v>
       </c>
@@ -4736,7 +4744,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="30" t="s">
         <v>561</v>
       </c>
@@ -4750,7 +4758,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="30" t="s">
         <v>571</v>
       </c>
@@ -4764,7 +4772,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="18" t="s">
         <v>564</v>
       </c>
@@ -4778,7 +4786,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
         <v>565</v>
       </c>
@@ -4792,7 +4800,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
         <v>566</v>
       </c>
@@ -4806,7 +4814,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="18" t="s">
         <v>567</v>
       </c>
@@ -4820,7 +4828,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="18" t="s">
         <v>568</v>
       </c>
@@ -4837,7 +4845,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="18" t="s">
         <v>569</v>
       </c>
@@ -4854,7 +4862,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="18" t="s">
         <v>570</v>
       </c>
@@ -4871,7 +4879,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="18" t="s">
         <v>860</v>
       </c>
@@ -4885,7 +4893,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="18" t="s">
         <v>941</v>
       </c>
@@ -4899,7 +4907,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="18" t="s">
         <v>866</v>
       </c>
@@ -4913,7 +4921,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="18" t="s">
         <v>584</v>
       </c>
@@ -4927,7 +4935,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="43" t="s">
         <v>580</v>
       </c>
@@ -4943,7 +4951,7 @@
       </c>
       <c r="M50" s="25"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="43" t="s">
         <v>939</v>
       </c>
@@ -4959,7 +4967,7 @@
       </c>
       <c r="M51" s="25"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="44" t="s">
         <v>949</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="44" t="s">
         <v>585</v>
       </c>
@@ -4993,7 +5001,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="44" t="s">
         <v>586</v>
       </c>
@@ -5010,7 +5018,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="44" t="s">
         <v>598</v>
       </c>
@@ -5027,7 +5035,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="44" t="s">
         <v>599</v>
       </c>
@@ -5044,7 +5052,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="44" t="s">
         <v>868</v>
       </c>
@@ -5061,7 +5069,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="44" t="s">
         <v>874</v>
       </c>
@@ -5078,7 +5086,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="44" t="s">
         <v>876</v>
       </c>
@@ -5095,7 +5103,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="44" t="s">
         <v>878</v>
       </c>
@@ -5112,7 +5120,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="44" t="s">
         <v>879</v>
       </c>
@@ -5129,7 +5137,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="44" t="s">
         <v>880</v>
       </c>
@@ -5146,7 +5154,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="44" t="s">
         <v>888</v>
       </c>
@@ -5163,7 +5171,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="44" t="s">
         <v>889</v>
       </c>
@@ -5180,7 +5188,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="44" t="s">
         <v>890</v>
       </c>
@@ -5197,7 +5205,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="44" t="s">
         <v>891</v>
       </c>
@@ -5214,7 +5222,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="44" t="s">
         <v>892</v>
       </c>
@@ -5231,7 +5239,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="44" t="s">
         <v>893</v>
       </c>
@@ -5248,7 +5256,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="44" t="s">
         <v>900</v>
       </c>
@@ -5265,7 +5273,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="44" t="s">
         <v>901</v>
       </c>
@@ -5282,7 +5290,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="44" t="s">
         <v>902</v>
       </c>
@@ -5299,7 +5307,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="44" t="s">
         <v>903</v>
       </c>
@@ -5316,7 +5324,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="44" t="s">
         <v>904</v>
       </c>
@@ -5333,7 +5341,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="44" t="s">
         <v>905</v>
       </c>
@@ -5350,7 +5358,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="44" t="s">
         <v>912</v>
       </c>
@@ -5367,7 +5375,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="44" t="s">
         <v>914</v>
       </c>
@@ -5384,7 +5392,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" s="44" t="s">
         <v>916</v>
       </c>
@@ -5401,7 +5409,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" s="44" t="s">
         <v>917</v>
       </c>
@@ -5418,7 +5426,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" s="44" t="s">
         <v>918</v>
       </c>
@@ -5435,7 +5443,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" s="44" t="s">
         <v>587</v>
       </c>
@@ -5452,7 +5460,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="81" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" customFormat="1">
       <c r="A81" s="41" t="s">
         <v>582</v>
       </c>
@@ -5469,7 +5477,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" s="18" t="s">
         <v>1067</v>
       </c>
@@ -5483,7 +5491,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" s="18" t="s">
         <v>1081</v>
       </c>
@@ -5497,7 +5505,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" s="18" t="s">
         <v>1068</v>
       </c>
@@ -5511,7 +5519,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13">
       <c r="A85" s="18" t="s">
         <v>1082</v>
       </c>
@@ -5525,7 +5533,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13">
       <c r="A86" s="18" t="s">
         <v>1069</v>
       </c>
@@ -5539,7 +5547,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="A87" s="18" t="s">
         <v>1083</v>
       </c>
@@ -5553,7 +5561,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="A88" s="18" t="s">
         <v>1070</v>
       </c>
@@ -5567,7 +5575,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="A89" s="18" t="s">
         <v>1084</v>
       </c>
@@ -5581,7 +5589,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" s="18" t="s">
         <v>1071</v>
       </c>
@@ -5595,7 +5603,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" s="18" t="s">
         <v>1085</v>
       </c>
@@ -5609,7 +5617,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" s="18" t="s">
         <v>1072</v>
       </c>
@@ -5623,7 +5631,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" s="18" t="s">
         <v>1086</v>
       </c>
@@ -5637,7 +5645,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="A94" s="18" t="s">
         <v>1073</v>
       </c>
@@ -5651,7 +5659,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13">
       <c r="A95" s="18" t="s">
         <v>1087</v>
       </c>
@@ -5665,7 +5673,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="18" t="s">
         <v>1074</v>
       </c>
@@ -5679,7 +5687,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="18" t="s">
         <v>1088</v>
       </c>
@@ -5693,7 +5701,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="18" t="s">
         <v>1075</v>
       </c>
@@ -5707,7 +5715,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="18" t="s">
         <v>1089</v>
       </c>
@@ -5721,7 +5729,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="18" t="s">
         <v>1076</v>
       </c>
@@ -5735,7 +5743,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" s="18" t="s">
         <v>1090</v>
       </c>
@@ -5749,7 +5757,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="18" t="s">
         <v>1077</v>
       </c>
@@ -5763,7 +5771,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="18" t="s">
         <v>1091</v>
       </c>
@@ -5777,7 +5785,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="18" t="s">
         <v>1078</v>
       </c>
@@ -5791,7 +5799,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="18" t="s">
         <v>1092</v>
       </c>
@@ -5805,7 +5813,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="18" t="s">
         <v>1079</v>
       </c>
@@ -5819,7 +5827,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="18" t="s">
         <v>1093</v>
       </c>
@@ -5833,7 +5841,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="18" t="s">
         <v>1080</v>
       </c>
@@ -5847,7 +5855,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" s="18" t="s">
         <v>1094</v>
       </c>
@@ -5861,7 +5869,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="18" t="s">
         <v>1095</v>
       </c>
@@ -5892,88 +5900,88 @@
   </sheetPr>
   <dimension ref="A1:CK32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="18" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="21" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="17" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="15" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="25" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="20" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="20" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="17" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="89" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="89" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" s="2" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -6242,7 +6250,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:89" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" s="12" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>219</v>
       </c>
@@ -6310,7 +6318,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89">
       <c r="A3" s="9" t="s">
         <v>220</v>
       </c>
@@ -6363,7 +6371,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89">
       <c r="A4" s="23" t="s">
         <v>383</v>
       </c>
@@ -6425,7 +6433,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89">
       <c r="A5" s="9" t="s">
         <v>221</v>
       </c>
@@ -6469,7 +6477,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89">
       <c r="A6" s="9" t="s">
         <v>386</v>
       </c>
@@ -6504,7 +6512,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89">
       <c r="A7" s="9" t="s">
         <v>384</v>
       </c>
@@ -6539,7 +6547,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89">
       <c r="A8" s="11" t="s">
         <v>385</v>
       </c>
@@ -6574,7 +6582,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89">
       <c r="A9" s="9" t="s">
         <v>222</v>
       </c>
@@ -6615,7 +6623,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89">
       <c r="A10" s="9" t="s">
         <v>223</v>
       </c>
@@ -6656,7 +6664,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89">
       <c r="A11" s="9" t="s">
         <v>224</v>
       </c>
@@ -6715,7 +6723,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89">
       <c r="A12" s="22" t="s">
         <v>226</v>
       </c>
@@ -6942,7 +6950,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89">
       <c r="A13" s="22" t="s">
         <v>225</v>
       </c>
@@ -6983,7 +6991,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89">
       <c r="A14" s="30" t="s">
         <v>339</v>
       </c>
@@ -7027,7 +7035,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89">
       <c r="A15" s="30" t="s">
         <v>351</v>
       </c>
@@ -7038,7 +7046,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89">
       <c r="A16" s="30" t="s">
         <v>352</v>
       </c>
@@ -7049,7 +7057,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
         <v>568</v>
       </c>
@@ -7060,7 +7068,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="30" t="s">
         <v>580</v>
       </c>
@@ -7086,7 +7094,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="30" t="s">
         <v>846</v>
       </c>
@@ -7097,7 +7105,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="30" t="s">
         <v>847</v>
       </c>
@@ -7108,7 +7116,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="30" t="s">
         <v>848</v>
       </c>
@@ -7119,7 +7127,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="30" t="s">
         <v>849</v>
       </c>
@@ -7130,7 +7138,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="30" t="s">
         <v>850</v>
       </c>
@@ -7141,7 +7149,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="30" t="s">
         <v>851</v>
       </c>
@@ -7152,7 +7160,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="18" t="s">
         <v>868</v>
       </c>
@@ -7169,7 +7177,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="18" t="s">
         <v>878</v>
       </c>
@@ -7189,7 +7197,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
         <v>888</v>
       </c>
@@ -7206,7 +7214,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
         <v>891</v>
       </c>
@@ -7226,7 +7234,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="18" t="s">
         <v>900</v>
       </c>
@@ -7243,7 +7251,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
         <v>903</v>
       </c>
@@ -7263,7 +7271,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>582</v>
       </c>
@@ -7280,7 +7288,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="30" t="s">
         <v>939</v>
       </c>
@@ -7319,25 +7327,25 @@
   </sheetPr>
   <dimension ref="A1:CK107"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:B107"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="53.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="6.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="89" width="7.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="90" max="1025" width="20.140625" style="18"/>
-    <col min="1026" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="53.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="6.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="89" width="7.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="90" max="1025" width="20.1796875" style="18"/>
+    <col min="1026" max="16384" width="9.1796875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -7606,7 +7614,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89">
       <c r="A2" s="9" t="s">
         <v>219</v>
       </c>
@@ -7678,7 +7686,7 @@
       <c r="Y2" s="17"/>
       <c r="Z2" s="17"/>
     </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89">
       <c r="A3" s="9" t="s">
         <v>220</v>
       </c>
@@ -7731,7 +7739,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89">
       <c r="A4" s="9" t="s">
         <v>383</v>
       </c>
@@ -7793,7 +7801,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89">
       <c r="A5" s="9" t="s">
         <v>221</v>
       </c>
@@ -7837,7 +7845,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89">
       <c r="A6" s="9" t="s">
         <v>386</v>
       </c>
@@ -7872,7 +7880,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89">
       <c r="A7" s="9" t="s">
         <v>384</v>
       </c>
@@ -7907,7 +7915,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89">
       <c r="A8" s="11" t="s">
         <v>385</v>
       </c>
@@ -7942,7 +7950,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89">
       <c r="A9" s="9" t="s">
         <v>222</v>
       </c>
@@ -7983,7 +7991,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89">
       <c r="A10" s="9" t="s">
         <v>223</v>
       </c>
@@ -8024,7 +8032,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89">
       <c r="A11" s="9" t="s">
         <v>224</v>
       </c>
@@ -8083,7 +8091,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89">
       <c r="A12" s="22" t="s">
         <v>226</v>
       </c>
@@ -8310,7 +8318,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89">
       <c r="A13" s="22" t="s">
         <v>225</v>
       </c>
@@ -8351,7 +8359,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89">
       <c r="A14" s="30" t="s">
         <v>339</v>
       </c>
@@ -8395,7 +8403,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89">
       <c r="A15" s="30" t="s">
         <v>351</v>
       </c>
@@ -8406,7 +8414,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89">
       <c r="A16" s="30" t="s">
         <v>352</v>
       </c>
@@ -8417,7 +8425,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="30" t="s">
         <v>846</v>
       </c>
@@ -8428,7 +8436,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="30" t="s">
         <v>847</v>
       </c>
@@ -8439,7 +8447,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="30" t="s">
         <v>848</v>
       </c>
@@ -8450,7 +8458,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="30" t="s">
         <v>849</v>
       </c>
@@ -8461,7 +8469,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="30" t="s">
         <v>850</v>
       </c>
@@ -8472,7 +8480,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="30" t="s">
         <v>851</v>
       </c>
@@ -8483,7 +8491,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="30" t="s">
         <v>375</v>
       </c>
@@ -8491,7 +8499,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="30" t="s">
         <v>340</v>
       </c>
@@ -8499,7 +8507,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="30" t="s">
         <v>342</v>
       </c>
@@ -8507,7 +8515,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="30" t="s">
         <v>343</v>
       </c>
@@ -8515,7 +8523,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="30" t="s">
         <v>344</v>
       </c>
@@ -8523,7 +8531,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="30" t="s">
         <v>345</v>
       </c>
@@ -8531,7 +8539,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="30" t="s">
         <v>943</v>
       </c>
@@ -8539,7 +8547,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="30" t="s">
         <v>942</v>
       </c>
@@ -8547,7 +8555,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="30" t="s">
         <v>557</v>
       </c>
@@ -8555,7 +8563,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="30" t="s">
         <v>558</v>
       </c>
@@ -8563,7 +8571,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="30" t="s">
         <v>559</v>
       </c>
@@ -8571,7 +8579,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="30" t="s">
         <v>562</v>
       </c>
@@ -8579,7 +8587,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="30" t="s">
         <v>560</v>
       </c>
@@ -8587,7 +8595,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="30" t="s">
         <v>561</v>
       </c>
@@ -8595,7 +8603,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="30" t="s">
         <v>571</v>
       </c>
@@ -8603,7 +8611,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="18" t="s">
         <v>564</v>
       </c>
@@ -8611,7 +8619,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="18" t="s">
         <v>565</v>
       </c>
@@ -8619,7 +8627,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="18" t="s">
         <v>566</v>
       </c>
@@ -8627,7 +8635,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="18" t="s">
         <v>567</v>
       </c>
@@ -8635,7 +8643,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="18" t="s">
         <v>568</v>
       </c>
@@ -8646,7 +8654,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="18" t="s">
         <v>569</v>
       </c>
@@ -8654,7 +8662,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="18" t="s">
         <v>570</v>
       </c>
@@ -8662,7 +8670,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="30" t="s">
         <v>580</v>
       </c>
@@ -8688,7 +8696,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="18" t="s">
         <v>860</v>
       </c>
@@ -8702,7 +8710,7 @@
       <c r="G46"/>
       <c r="H46"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="18" t="s">
         <v>941</v>
       </c>
@@ -8710,7 +8718,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="18" t="s">
         <v>585</v>
       </c>
@@ -8718,7 +8726,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="18" t="s">
         <v>586</v>
       </c>
@@ -8726,7 +8734,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="18" t="s">
         <v>598</v>
       </c>
@@ -8734,7 +8742,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="18" t="s">
         <v>599</v>
       </c>
@@ -8742,7 +8750,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="18" t="s">
         <v>868</v>
       </c>
@@ -8759,7 +8767,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="18" t="s">
         <v>874</v>
       </c>
@@ -8767,7 +8775,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="18" t="s">
         <v>876</v>
       </c>
@@ -8775,7 +8783,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="18" t="s">
         <v>878</v>
       </c>
@@ -8791,8 +8799,11 @@
       <c r="E55" s="18" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="18" t="s">
         <v>879</v>
       </c>
@@ -8800,7 +8811,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="18" t="s">
         <v>880</v>
       </c>
@@ -8808,7 +8819,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="18" t="s">
         <v>888</v>
       </c>
@@ -8825,7 +8836,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="18" t="s">
         <v>889</v>
       </c>
@@ -8833,7 +8844,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="18" t="s">
         <v>890</v>
       </c>
@@ -8841,7 +8852,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="18" t="s">
         <v>891</v>
       </c>
@@ -8857,8 +8868,11 @@
       <c r="E61" s="18" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="18" t="s">
         <v>892</v>
       </c>
@@ -8866,7 +8880,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="18" t="s">
         <v>893</v>
       </c>
@@ -8874,7 +8888,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="18" t="s">
         <v>900</v>
       </c>
@@ -8891,7 +8905,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="18" t="s">
         <v>901</v>
       </c>
@@ -8899,7 +8913,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="18" t="s">
         <v>902</v>
       </c>
@@ -8907,7 +8921,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="18" t="s">
         <v>903</v>
       </c>
@@ -8923,8 +8937,11 @@
       <c r="E67" s="18" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F67" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="18" t="s">
         <v>904</v>
       </c>
@@ -8932,7 +8949,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="18" t="s">
         <v>905</v>
       </c>
@@ -8940,7 +8957,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="18" t="s">
         <v>912</v>
       </c>
@@ -8948,7 +8965,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="18" t="s">
         <v>914</v>
       </c>
@@ -8956,7 +8973,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="18" t="s">
         <v>916</v>
       </c>
@@ -8964,7 +8981,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="18" t="s">
         <v>917</v>
       </c>
@@ -8972,7 +8989,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="18" t="s">
         <v>918</v>
       </c>
@@ -8980,7 +8997,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="18" t="s">
         <v>587</v>
       </c>
@@ -8988,7 +9005,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" customFormat="1">
       <c r="A76" t="s">
         <v>582</v>
       </c>
@@ -9005,7 +9022,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="30" t="s">
         <v>939</v>
       </c>
@@ -9031,7 +9048,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="18" t="s">
         <v>949</v>
       </c>
@@ -9039,7 +9056,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="18" t="s">
         <v>1067</v>
       </c>
@@ -9047,7 +9064,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="18" t="s">
         <v>1068</v>
       </c>
@@ -9055,7 +9072,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="18" t="s">
         <v>1069</v>
       </c>
@@ -9063,7 +9080,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="18" t="s">
         <v>1070</v>
       </c>
@@ -9071,7 +9088,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="18" t="s">
         <v>1071</v>
       </c>
@@ -9079,7 +9096,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="18" t="s">
         <v>1072</v>
       </c>
@@ -9087,7 +9104,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="18" t="s">
         <v>1073</v>
       </c>
@@ -9095,7 +9112,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="18" t="s">
         <v>1074</v>
       </c>
@@ -9103,7 +9120,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="18" t="s">
         <v>1075</v>
       </c>
@@ -9111,7 +9128,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="18" t="s">
         <v>1076</v>
       </c>
@@ -9119,7 +9136,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" s="18" t="s">
         <v>1077</v>
       </c>
@@ -9127,7 +9144,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="18" t="s">
         <v>1078</v>
       </c>
@@ -9135,7 +9152,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="18" t="s">
         <v>1079</v>
       </c>
@@ -9143,7 +9160,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" s="18" t="s">
         <v>1080</v>
       </c>
@@ -9151,7 +9168,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" s="18" t="s">
         <v>1081</v>
       </c>
@@ -9159,7 +9176,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="18" t="s">
         <v>1082</v>
       </c>
@@ -9167,7 +9184,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="18" t="s">
         <v>1083</v>
       </c>
@@ -9175,7 +9192,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="18" t="s">
         <v>1084</v>
       </c>
@@ -9183,7 +9200,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="18" t="s">
         <v>1085</v>
       </c>
@@ -9191,7 +9208,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="18" t="s">
         <v>1086</v>
       </c>
@@ -9199,7 +9216,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="18" t="s">
         <v>1087</v>
       </c>
@@ -9207,7 +9224,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="18" t="s">
         <v>1088</v>
       </c>
@@ -9215,7 +9232,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" s="18" t="s">
         <v>1089</v>
       </c>
@@ -9223,7 +9240,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="18" t="s">
         <v>1090</v>
       </c>
@@ -9231,7 +9248,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" s="18" t="s">
         <v>1091</v>
       </c>
@@ -9239,7 +9256,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2">
       <c r="A104" s="18" t="s">
         <v>1092</v>
       </c>
@@ -9247,7 +9264,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" s="18" t="s">
         <v>1093</v>
       </c>
@@ -9255,7 +9272,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" s="18" t="s">
         <v>1094</v>
       </c>
@@ -9263,7 +9280,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2">
       <c r="A107" s="18" t="s">
         <v>1095</v>
       </c>
@@ -9291,23 +9308,23 @@
       <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="53.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="6.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="6.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" style="21" bestFit="1" customWidth="1"/>
     <col min="11" max="22" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="73" width="7.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="9.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="76" max="89" width="7.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="90" max="1025" width="20.140625" style="21"/>
-    <col min="1026" max="16384" width="9.140625" style="21"/>
+    <col min="23" max="73" width="7.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="9.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="76" max="89" width="7.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="90" max="1025" width="20.1796875" style="21"/>
+    <col min="1026" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" s="20" customFormat="1">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
@@ -9576,7 +9593,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:89" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" s="10" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>219</v>
       </c>
@@ -9644,7 +9661,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:89" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" s="10" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>220</v>
       </c>
@@ -9701,7 +9718,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89">
       <c r="A4" s="23" t="s">
         <v>383</v>
       </c>
@@ -9763,7 +9780,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89">
       <c r="A5" s="9" t="s">
         <v>221</v>
       </c>
@@ -9807,7 +9824,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89">
       <c r="A6" s="9" t="s">
         <v>386</v>
       </c>
@@ -9842,7 +9859,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89">
       <c r="A7" s="9" t="s">
         <v>384</v>
       </c>
@@ -9877,7 +9894,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89">
       <c r="A8" s="11" t="s">
         <v>385</v>
       </c>
@@ -9912,7 +9929,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89">
       <c r="A9" s="9" t="s">
         <v>222</v>
       </c>
@@ -9953,7 +9970,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89">
       <c r="A10" s="9" t="s">
         <v>223</v>
       </c>
@@ -9994,7 +10011,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89">
       <c r="A11" s="9" t="s">
         <v>224</v>
       </c>
@@ -10053,7 +10070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89">
       <c r="A12" s="21" t="s">
         <v>226</v>
       </c>
@@ -10280,7 +10297,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89">
       <c r="A13" s="22" t="s">
         <v>225</v>
       </c>
@@ -10321,7 +10338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89">
       <c r="A14" s="30" t="s">
         <v>375</v>
       </c>
@@ -10329,7 +10346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89">
       <c r="A15" s="30" t="s">
         <v>340</v>
       </c>
@@ -10337,7 +10354,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89">
       <c r="A16" s="30" t="s">
         <v>342</v>
       </c>
@@ -10345,7 +10362,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="30" t="s">
         <v>343</v>
       </c>
@@ -10353,7 +10370,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="30" t="s">
         <v>344</v>
       </c>
@@ -10361,7 +10378,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="30" t="s">
         <v>345</v>
       </c>
@@ -10369,7 +10386,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="30" t="s">
         <v>943</v>
       </c>
@@ -10377,7 +10394,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="30" t="s">
         <v>942</v>
       </c>
@@ -10385,7 +10402,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="30" t="s">
         <v>557</v>
       </c>
@@ -10393,7 +10410,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" s="30" t="s">
         <v>562</v>
       </c>
@@ -10401,7 +10418,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="30" t="s">
         <v>560</v>
       </c>
@@ -10409,7 +10426,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="30" t="s">
         <v>561</v>
       </c>
@@ -10417,7 +10434,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="18" t="s">
         <v>564</v>
       </c>
@@ -10425,7 +10442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="18" t="s">
         <v>565</v>
       </c>
@@ -10433,7 +10450,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="18" t="s">
         <v>566</v>
       </c>
@@ -10441,7 +10458,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="18" t="s">
         <v>567</v>
       </c>
@@ -10449,7 +10466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="18" t="s">
         <v>568</v>
       </c>
@@ -10460,7 +10477,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="18" t="s">
         <v>569</v>
       </c>
@@ -10468,7 +10485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="18" t="s">
         <v>570</v>
       </c>
@@ -10476,7 +10493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="30" t="s">
         <v>580</v>
       </c>
@@ -10502,7 +10519,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
         <v>941</v>
       </c>
@@ -10510,7 +10527,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
         <v>586</v>
       </c>
@@ -10518,7 +10535,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="18" t="s">
         <v>599</v>
       </c>
@@ -10526,7 +10543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="18" t="s">
         <v>868</v>
       </c>
@@ -10543,7 +10560,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="18" t="s">
         <v>874</v>
       </c>
@@ -10551,7 +10568,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="18" t="s">
         <v>876</v>
       </c>
@@ -10559,7 +10576,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="18" t="s">
         <v>878</v>
       </c>
@@ -10579,7 +10596,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="18" t="s">
         <v>879</v>
       </c>
@@ -10587,7 +10604,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="18" t="s">
         <v>880</v>
       </c>
@@ -10595,7 +10612,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="18" t="s">
         <v>888</v>
       </c>
@@ -10612,7 +10629,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="18" t="s">
         <v>889</v>
       </c>
@@ -10620,7 +10637,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="18" t="s">
         <v>890</v>
       </c>
@@ -10628,7 +10645,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="18" t="s">
         <v>891</v>
       </c>
@@ -10648,7 +10665,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="18" t="s">
         <v>892</v>
       </c>
@@ -10656,7 +10673,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="18" t="s">
         <v>893</v>
       </c>
@@ -10664,7 +10681,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="18" t="s">
         <v>900</v>
       </c>
@@ -10681,7 +10698,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="18" t="s">
         <v>901</v>
       </c>
@@ -10689,7 +10706,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="18" t="s">
         <v>902</v>
       </c>
@@ -10697,7 +10714,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="18" t="s">
         <v>903</v>
       </c>
@@ -10717,7 +10734,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="18" t="s">
         <v>904</v>
       </c>
@@ -10725,7 +10742,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="18" t="s">
         <v>905</v>
       </c>
@@ -10733,7 +10750,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="18" t="s">
         <v>912</v>
       </c>
@@ -10741,7 +10758,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="18" t="s">
         <v>914</v>
       </c>
@@ -10749,7 +10766,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="18" t="s">
         <v>916</v>
       </c>
@@ -10757,7 +10774,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="18" t="s">
         <v>917</v>
       </c>
@@ -10765,7 +10782,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="18" t="s">
         <v>918</v>
       </c>
@@ -10773,7 +10790,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="18" t="s">
         <v>587</v>
       </c>
@@ -10781,7 +10798,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>582</v>
       </c>
@@ -10798,7 +10815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="30" t="s">
         <v>939</v>
       </c>
@@ -10824,7 +10841,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="18" t="s">
         <v>1081</v>
       </c>
@@ -10832,7 +10849,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="18" t="s">
         <v>1082</v>
       </c>
@@ -10840,7 +10857,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="18" t="s">
         <v>1083</v>
       </c>
@@ -10848,7 +10865,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="18" t="s">
         <v>1084</v>
       </c>
@@ -10856,7 +10873,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="18" t="s">
         <v>1085</v>
       </c>
@@ -10864,7 +10881,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="18" t="s">
         <v>1086</v>
       </c>
@@ -10872,7 +10889,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="18" t="s">
         <v>1087</v>
       </c>
@@ -10880,7 +10897,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="18" t="s">
         <v>1088</v>
       </c>
@@ -10888,7 +10905,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="18" t="s">
         <v>1089</v>
       </c>
@@ -10896,7 +10913,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="18" t="s">
         <v>1090</v>
       </c>
@@ -10904,7 +10921,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="18" t="s">
         <v>1091</v>
       </c>
@@ -10912,7 +10929,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="18" t="s">
         <v>1092</v>
       </c>
@@ -10920,7 +10937,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="18" t="s">
         <v>1093</v>
       </c>
@@ -10928,7 +10945,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="18" t="s">
         <v>1094</v>
       </c>
@@ -10953,15 +10970,15 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.85546875"/>
-    <col min="2" max="2" width="20.140625"/>
-    <col min="3" max="3" width="24.28515625"/>
-    <col min="4" max="1025" width="20.140625"/>
+    <col min="1" max="1" width="33.81640625"/>
+    <col min="2" max="2" width="20.1796875"/>
+    <col min="3" max="3" width="24.26953125"/>
+    <col min="4" max="1025" width="20.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" s="2" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -10979,7 +10996,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:76">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -11050,7 +11067,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76">
       <c r="A3" t="s">
         <v>220</v>
       </c>
@@ -11106,7 +11123,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76">
       <c r="A4" t="s">
         <v>383</v>
       </c>
@@ -11171,7 +11188,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -11218,7 +11235,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76">
       <c r="A6" t="s">
         <v>386</v>
       </c>
@@ -11256,7 +11273,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76">
       <c r="A7" t="s">
         <v>384</v>
       </c>
@@ -11294,7 +11311,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76">
       <c r="A8" t="s">
         <v>385</v>
       </c>
@@ -11332,7 +11349,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -11376,7 +11393,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:76">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -11420,7 +11437,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -11482,7 +11499,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -11712,7 +11729,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -11756,7 +11773,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76">
       <c r="A14" t="s">
         <v>568</v>
       </c>
@@ -11776,7 +11793,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76">
       <c r="A15" t="s">
         <v>569</v>
       </c>
@@ -11793,7 +11810,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76">
       <c r="A16" t="s">
         <v>570</v>
       </c>
@@ -11810,7 +11827,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="30" t="s">
         <v>863</v>
       </c>
@@ -11841,26 +11858,26 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="1025" width="20.140625"/>
+    <col min="1" max="1" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="20.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -11877,7 +11894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="4" customFormat="1">
       <c r="A2" s="30" t="s">
         <v>351</v>
       </c>
@@ -11890,7 +11907,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1">
       <c r="A3" s="30" t="s">
         <v>352</v>
       </c>
@@ -11936,7 +11953,7 @@
       <c r="O3"/>
       <c r="P3"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="4" customFormat="1">
       <c r="A4" s="30" t="s">
         <v>846</v>
       </c>
@@ -11960,7 +11977,7 @@
       <c r="O4"/>
       <c r="P4"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="4" customFormat="1">
       <c r="A5" s="30" t="s">
         <v>847</v>
       </c>
@@ -11982,7 +11999,7 @@
       <c r="O5"/>
       <c r="P5"/>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="4" customFormat="1">
       <c r="A6" s="30" t="s">
         <v>848</v>
       </c>
@@ -12004,7 +12021,7 @@
       <c r="O6"/>
       <c r="P6"/>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="4" customFormat="1">
       <c r="A7" s="30" t="s">
         <v>849</v>
       </c>
@@ -12030,7 +12047,7 @@
       <c r="O7"/>
       <c r="P7"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="4" customFormat="1">
       <c r="A8" s="30" t="s">
         <v>850</v>
       </c>
@@ -12062,7 +12079,7 @@
       <c r="O8"/>
       <c r="P8"/>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="4" customFormat="1">
       <c r="A9" s="30" t="s">
         <v>851</v>
       </c>
@@ -12086,7 +12103,7 @@
       <c r="O9"/>
       <c r="P9"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="18" t="s">
         <v>860</v>
       </c>
@@ -12097,7 +12114,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="30" t="s">
         <v>559</v>
       </c>
@@ -12108,7 +12125,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="30" t="s">
         <v>558</v>
       </c>
@@ -12125,7 +12142,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="30" t="s">
         <v>580</v>
       </c>
@@ -12139,7 +12156,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="30" t="s">
         <v>939</v>
       </c>
@@ -12147,7 +12164,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="30" t="s">
         <v>339</v>
       </c>
@@ -12181,13 +12198,13 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="11.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.453125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="10:26">
       <c r="J1" s="7"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>

</xml_diff>

<commit_message>
Fix bugs with database read.
</commit_message>
<xml_diff>
--- a/dds/installation.xlsx
+++ b/dds/installation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="590" yWindow="1010" windowWidth="10210" windowHeight="6080" tabRatio="474" activeTab="3"/>
+    <workbookView xWindow="590" yWindow="1010" windowWidth="10210" windowHeight="6080" tabRatio="474"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3037" uniqueCount="806">
   <si>
     <t>Identifier</t>
   </si>
@@ -1984,9 +1984,6 @@
     <t>Depth Rating</t>
   </si>
   <si>
-    <t xml:space="preserve">equipment_day_rate </t>
-  </si>
-  <si>
     <t>Min Pile Diameter</t>
   </si>
   <si>
@@ -2450,6 +2447,9 @@
   </si>
   <si>
     <t>l/hour</t>
+  </si>
+  <si>
+    <t>hidden.device_filtered</t>
   </si>
 </sst>
 </file>
@@ -3132,9 +3132,9 @@
   </sheetPr>
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3145,7 +3145,7 @@
     <col min="4" max="4" width="91.08984375" style="48" customWidth="1"/>
     <col min="5" max="5" width="13.90625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" style="13" customWidth="1"/>
     <col min="8" max="8" width="15.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="1021" width="20.1796875" style="13"/>
     <col min="1022" max="16384" width="9.1796875" style="13"/>
@@ -3395,16 +3395,16 @@
     </row>
     <row r="14" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="39" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="15" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="39" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C15" s="40" t="s">
+        <v>710</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>711</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>712</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
@@ -3431,16 +3431,16 @@
     </row>
     <row r="16" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="39" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C16" s="40" t="s">
+        <v>717</v>
+      </c>
+      <c r="D16" s="44" t="s">
         <v>718</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>719</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
@@ -3449,16 +3449,16 @@
     </row>
     <row r="17" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C17" s="40" t="s">
+        <v>737</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>738</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>739</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
@@ -3467,16 +3467,16 @@
     </row>
     <row r="18" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="39" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C18" s="40" t="s">
+        <v>742</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>743</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>744</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -3485,16 +3485,16 @@
     </row>
     <row r="19" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="39" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C19" s="40" t="s">
+        <v>722</v>
+      </c>
+      <c r="D19" s="44" t="s">
         <v>723</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>724</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -3503,16 +3503,16 @@
     </row>
     <row r="20" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="39" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C20" s="40" t="s">
+        <v>726</v>
+      </c>
+      <c r="D20" s="44" t="s">
         <v>727</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>728</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -3521,16 +3521,16 @@
     </row>
     <row r="21" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="39" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -3539,16 +3539,16 @@
     </row>
     <row r="22" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="39" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C22" s="40" t="s">
+        <v>733</v>
+      </c>
+      <c r="D22" s="44" t="s">
         <v>734</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>735</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -3557,16 +3557,16 @@
     </row>
     <row r="23" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="39" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C23" s="40" t="s">
+        <v>746</v>
+      </c>
+      <c r="D23" s="44" t="s">
         <v>747</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>748</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -3575,16 +3575,16 @@
     </row>
     <row r="24" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C24" s="40" t="s">
+        <v>750</v>
+      </c>
+      <c r="D24" s="44" t="s">
         <v>751</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>752</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -3593,16 +3593,16 @@
     </row>
     <row r="25" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -3611,16 +3611,16 @@
     </row>
     <row r="26" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="39" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C26" s="40" t="s">
+        <v>754</v>
+      </c>
+      <c r="D26" s="44" t="s">
         <v>755</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>756</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -3658,6 +3658,9 @@
       <c r="D28" s="42" t="s">
         <v>386</v>
       </c>
+      <c r="G28" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="29" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="31" t="s">
@@ -3672,6 +3675,9 @@
       <c r="D29" s="42" t="s">
         <v>417</v>
       </c>
+      <c r="G29" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="30" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
@@ -3686,6 +3692,9 @@
       <c r="D30" s="42" t="s">
         <v>434</v>
       </c>
+      <c r="G30" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="31" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="34" t="s">
@@ -3702,7 +3711,9 @@
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="32" t="s">
+        <v>805</v>
+      </c>
       <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
@@ -3718,6 +3729,9 @@
       <c r="D32" s="42" t="s">
         <v>435</v>
       </c>
+      <c r="G32" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="31" t="s">
@@ -3732,6 +3746,9 @@
       <c r="D33" s="42" t="s">
         <v>415</v>
       </c>
+      <c r="G33" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="34" spans="1:8" s="32" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="34" t="s">
@@ -3748,7 +3765,9 @@
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="32" t="s">
+        <v>805</v>
+      </c>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
@@ -3764,6 +3783,9 @@
       <c r="D35" s="42" t="s">
         <v>416</v>
       </c>
+      <c r="G35" s="32" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="36" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="31" t="s">
@@ -3780,7 +3802,9 @@
       </c>
       <c r="E36" s="32"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
+      <c r="G36" s="32" t="s">
+        <v>805</v>
+      </c>
       <c r="H36" s="32"/>
     </row>
     <row r="37" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4231,7 +4255,7 @@
         <v>463</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>507</v>
@@ -4263,7 +4287,7 @@
         <v>466</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>510</v>
@@ -4291,7 +4315,7 @@
         <v>460</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>504</v>
@@ -4319,7 +4343,7 @@
         <v>468</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>512</v>
@@ -4347,7 +4371,7 @@
         <v>471</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C69" s="26" t="s">
         <v>515</v>
@@ -4375,7 +4399,7 @@
         <v>467</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C71" s="26" t="s">
         <v>511</v>
@@ -4403,7 +4427,7 @@
         <v>461</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>505</v>
@@ -4431,7 +4455,7 @@
         <v>462</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>506</v>
@@ -4459,7 +4483,7 @@
         <v>469</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C77" s="26" t="s">
         <v>513</v>
@@ -4491,7 +4515,7 @@
         <v>470</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C79" s="26" t="s">
         <v>514</v>
@@ -4519,7 +4543,7 @@
         <v>465</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C81" s="26" t="s">
         <v>509</v>
@@ -4555,7 +4579,7 @@
         <v>472</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>516</v>
@@ -4591,7 +4615,7 @@
         <v>459</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>503</v>
@@ -4623,7 +4647,7 @@
         <v>464</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C87" s="26" t="s">
         <v>508</v>
@@ -5586,10 +5610,10 @@
         <v>649</v>
       </c>
       <c r="F7" t="s">
+        <v>650</v>
+      </c>
+      <c r="G7" t="s">
         <v>651</v>
-      </c>
-      <c r="G7" t="s">
-        <v>652</v>
       </c>
       <c r="H7" t="s">
         <v>636</v>
@@ -5618,7 +5642,7 @@
         <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F8" t="s">
         <v>174</v>
@@ -5638,31 +5662,31 @@
         <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E9" t="s">
+        <v>669</v>
+      </c>
+      <c r="F9" t="s">
         <v>670</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>671</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>672</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>673</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>674</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>675</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>676</v>
-      </c>
-      <c r="L9" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
@@ -5693,7 +5717,7 @@
         <v>135</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D11" t="s">
         <v>133</v>
@@ -5714,7 +5738,7 @@
         <v>144</v>
       </c>
       <c r="J11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K11" t="s">
         <v>636</v>
@@ -5723,19 +5747,19 @@
         <v>648</v>
       </c>
       <c r="M11" t="s">
+        <v>655</v>
+      </c>
+      <c r="N11" t="s">
         <v>656</v>
-      </c>
-      <c r="N11" t="s">
-        <v>657</v>
       </c>
       <c r="O11" t="s">
         <v>637</v>
       </c>
       <c r="P11" t="s">
+        <v>660</v>
+      </c>
+      <c r="Q11" t="s">
         <v>661</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
@@ -5754,13 +5778,13 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B13" t="s">
         <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D13" t="s">
         <v>131</v>
@@ -5769,57 +5793,57 @@
         <v>143</v>
       </c>
       <c r="F13" t="s">
+        <v>698</v>
+      </c>
+      <c r="G13" t="s">
         <v>699</v>
       </c>
-      <c r="G13" t="s">
-        <v>700</v>
-      </c>
       <c r="H13" t="s">
+        <v>759</v>
+      </c>
+      <c r="I13" t="s">
         <v>760</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>761</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>701</v>
+      </c>
+      <c r="L13" t="s">
         <v>762</v>
       </c>
-      <c r="K13" t="s">
-        <v>702</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>763</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>764</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>765</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>695</v>
+      </c>
+      <c r="R13" t="s">
+        <v>776</v>
+      </c>
+      <c r="S13" t="s">
         <v>766</v>
-      </c>
-      <c r="P13" t="s">
-        <v>697</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>696</v>
-      </c>
-      <c r="R13" t="s">
-        <v>777</v>
-      </c>
-      <c r="S13" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B14" t="s">
         <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D14" t="s">
         <v>131</v>
@@ -5828,78 +5852,78 @@
         <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
       </c>
       <c r="H14" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I14" t="s">
+        <v>698</v>
+      </c>
+      <c r="J14" t="s">
         <v>699</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>759</v>
+      </c>
+      <c r="L14" t="s">
+        <v>760</v>
+      </c>
+      <c r="M14" t="s">
+        <v>761</v>
+      </c>
+      <c r="N14" t="s">
         <v>700</v>
       </c>
-      <c r="K14" t="s">
-        <v>760</v>
-      </c>
-      <c r="L14" t="s">
-        <v>761</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
+        <v>706</v>
+      </c>
+      <c r="P14" t="s">
+        <v>757</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>701</v>
+      </c>
+      <c r="R14" t="s">
+        <v>768</v>
+      </c>
+      <c r="S14" t="s">
         <v>762</v>
       </c>
-      <c r="N14" t="s">
-        <v>701</v>
-      </c>
-      <c r="O14" t="s">
-        <v>707</v>
-      </c>
-      <c r="P14" t="s">
-        <v>758</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>702</v>
-      </c>
-      <c r="R14" t="s">
-        <v>769</v>
-      </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>763</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>764</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>765</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
+        <v>696</v>
+      </c>
+      <c r="X14" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>776</v>
+      </c>
+      <c r="Z14" t="s">
         <v>766</v>
-      </c>
-      <c r="W14" t="s">
-        <v>697</v>
-      </c>
-      <c r="X14" t="s">
-        <v>696</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>777</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B15" t="s">
         <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D15" t="s">
         <v>131</v>
@@ -5908,78 +5932,78 @@
         <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G15" t="s">
         <v>143</v>
       </c>
       <c r="H15" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I15" t="s">
+        <v>698</v>
+      </c>
+      <c r="J15" t="s">
         <v>699</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
+        <v>759</v>
+      </c>
+      <c r="L15" t="s">
+        <v>760</v>
+      </c>
+      <c r="M15" t="s">
+        <v>761</v>
+      </c>
+      <c r="N15" t="s">
         <v>700</v>
       </c>
-      <c r="K15" t="s">
-        <v>760</v>
-      </c>
-      <c r="L15" t="s">
-        <v>761</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
+        <v>706</v>
+      </c>
+      <c r="P15" t="s">
+        <v>757</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>701</v>
+      </c>
+      <c r="R15" t="s">
+        <v>768</v>
+      </c>
+      <c r="S15" t="s">
         <v>762</v>
       </c>
-      <c r="N15" t="s">
-        <v>701</v>
-      </c>
-      <c r="O15" t="s">
-        <v>707</v>
-      </c>
-      <c r="P15" t="s">
-        <v>758</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>702</v>
-      </c>
-      <c r="R15" t="s">
-        <v>769</v>
-      </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>763</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>764</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>765</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
+        <v>696</v>
+      </c>
+      <c r="X15" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>776</v>
+      </c>
+      <c r="Z15" t="s">
         <v>766</v>
-      </c>
-      <c r="W15" t="s">
-        <v>697</v>
-      </c>
-      <c r="X15" t="s">
-        <v>696</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>777</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B16" t="s">
         <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D16" t="s">
         <v>131</v>
@@ -5988,66 +6012,66 @@
         <v>142</v>
       </c>
       <c r="F16" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G16" t="s">
         <v>143</v>
       </c>
       <c r="H16" t="s">
+        <v>698</v>
+      </c>
+      <c r="I16" t="s">
         <v>699</v>
       </c>
-      <c r="I16" t="s">
-        <v>700</v>
-      </c>
       <c r="J16" t="s">
+        <v>759</v>
+      </c>
+      <c r="K16" t="s">
         <v>760</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>761</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
+        <v>704</v>
+      </c>
+      <c r="N16" t="s">
+        <v>701</v>
+      </c>
+      <c r="O16" t="s">
         <v>762</v>
       </c>
-      <c r="M16" t="s">
-        <v>705</v>
-      </c>
-      <c r="N16" t="s">
-        <v>702</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>763</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>764</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>765</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
+        <v>696</v>
+      </c>
+      <c r="T16" t="s">
+        <v>695</v>
+      </c>
+      <c r="U16" t="s">
+        <v>776</v>
+      </c>
+      <c r="V16" t="s">
         <v>766</v>
-      </c>
-      <c r="S16" t="s">
-        <v>697</v>
-      </c>
-      <c r="T16" t="s">
-        <v>696</v>
-      </c>
-      <c r="U16" t="s">
-        <v>777</v>
-      </c>
-      <c r="V16" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B17" t="s">
         <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D17" t="s">
         <v>131</v>
@@ -6056,66 +6080,66 @@
         <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G17" t="s">
         <v>143</v>
       </c>
       <c r="H17" t="s">
+        <v>698</v>
+      </c>
+      <c r="I17" t="s">
         <v>699</v>
       </c>
-      <c r="I17" t="s">
-        <v>700</v>
-      </c>
       <c r="J17" t="s">
+        <v>759</v>
+      </c>
+      <c r="K17" t="s">
         <v>760</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>761</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
+        <v>704</v>
+      </c>
+      <c r="N17" t="s">
+        <v>701</v>
+      </c>
+      <c r="O17" t="s">
         <v>762</v>
       </c>
-      <c r="M17" t="s">
-        <v>705</v>
-      </c>
-      <c r="N17" t="s">
-        <v>702</v>
-      </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>763</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>764</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>765</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
+        <v>696</v>
+      </c>
+      <c r="T17" t="s">
+        <v>695</v>
+      </c>
+      <c r="U17" t="s">
+        <v>776</v>
+      </c>
+      <c r="V17" t="s">
         <v>766</v>
-      </c>
-      <c r="S17" t="s">
-        <v>697</v>
-      </c>
-      <c r="T17" t="s">
-        <v>696</v>
-      </c>
-      <c r="U17" t="s">
-        <v>777</v>
-      </c>
-      <c r="V17" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B18" t="s">
         <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -6124,66 +6148,66 @@
         <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G18" t="s">
         <v>143</v>
       </c>
       <c r="H18" t="s">
+        <v>698</v>
+      </c>
+      <c r="I18" t="s">
         <v>699</v>
       </c>
-      <c r="I18" t="s">
-        <v>700</v>
-      </c>
       <c r="J18" t="s">
+        <v>759</v>
+      </c>
+      <c r="K18" t="s">
         <v>760</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>761</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
+        <v>704</v>
+      </c>
+      <c r="N18" t="s">
+        <v>701</v>
+      </c>
+      <c r="O18" t="s">
         <v>762</v>
       </c>
-      <c r="M18" t="s">
-        <v>705</v>
-      </c>
-      <c r="N18" t="s">
-        <v>702</v>
-      </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>763</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>764</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>765</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
+        <v>696</v>
+      </c>
+      <c r="T18" t="s">
+        <v>695</v>
+      </c>
+      <c r="U18" t="s">
+        <v>776</v>
+      </c>
+      <c r="V18" t="s">
         <v>766</v>
-      </c>
-      <c r="S18" t="s">
-        <v>697</v>
-      </c>
-      <c r="T18" t="s">
-        <v>696</v>
-      </c>
-      <c r="U18" t="s">
-        <v>777</v>
-      </c>
-      <c r="V18" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B19" t="s">
         <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D19" t="s">
         <v>131</v>
@@ -6192,66 +6216,66 @@
         <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G19" t="s">
         <v>143</v>
       </c>
       <c r="H19" t="s">
+        <v>698</v>
+      </c>
+      <c r="I19" t="s">
         <v>699</v>
       </c>
-      <c r="I19" t="s">
-        <v>700</v>
-      </c>
       <c r="J19" t="s">
+        <v>759</v>
+      </c>
+      <c r="K19" t="s">
         <v>760</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>761</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
+        <v>704</v>
+      </c>
+      <c r="N19" t="s">
+        <v>701</v>
+      </c>
+      <c r="O19" t="s">
         <v>762</v>
       </c>
-      <c r="M19" t="s">
-        <v>705</v>
-      </c>
-      <c r="N19" t="s">
-        <v>702</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>763</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>764</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>765</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
+        <v>696</v>
+      </c>
+      <c r="T19" t="s">
+        <v>695</v>
+      </c>
+      <c r="U19" t="s">
+        <v>776</v>
+      </c>
+      <c r="V19" t="s">
         <v>766</v>
-      </c>
-      <c r="S19" t="s">
-        <v>697</v>
-      </c>
-      <c r="T19" t="s">
-        <v>696</v>
-      </c>
-      <c r="U19" t="s">
-        <v>777</v>
-      </c>
-      <c r="V19" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B20" t="s">
         <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -6260,66 +6284,66 @@
         <v>142</v>
       </c>
       <c r="F20" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G20" t="s">
         <v>143</v>
       </c>
       <c r="H20" t="s">
+        <v>698</v>
+      </c>
+      <c r="I20" t="s">
         <v>699</v>
       </c>
-      <c r="I20" t="s">
-        <v>700</v>
-      </c>
       <c r="J20" t="s">
+        <v>759</v>
+      </c>
+      <c r="K20" t="s">
         <v>760</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>761</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
+        <v>704</v>
+      </c>
+      <c r="N20" t="s">
+        <v>701</v>
+      </c>
+      <c r="O20" t="s">
         <v>762</v>
       </c>
-      <c r="M20" t="s">
-        <v>705</v>
-      </c>
-      <c r="N20" t="s">
-        <v>702</v>
-      </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>763</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>764</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>765</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
+        <v>696</v>
+      </c>
+      <c r="T20" t="s">
+        <v>695</v>
+      </c>
+      <c r="U20" t="s">
+        <v>776</v>
+      </c>
+      <c r="V20" t="s">
         <v>766</v>
-      </c>
-      <c r="S20" t="s">
-        <v>697</v>
-      </c>
-      <c r="T20" t="s">
-        <v>696</v>
-      </c>
-      <c r="U20" t="s">
-        <v>777</v>
-      </c>
-      <c r="V20" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B21" t="s">
         <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D21" t="s">
         <v>131</v>
@@ -6328,78 +6352,78 @@
         <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G21" t="s">
         <v>143</v>
       </c>
       <c r="H21" t="s">
+        <v>698</v>
+      </c>
+      <c r="I21" t="s">
         <v>699</v>
       </c>
-      <c r="I21" t="s">
-        <v>700</v>
-      </c>
       <c r="J21" t="s">
+        <v>759</v>
+      </c>
+      <c r="K21" t="s">
         <v>760</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>761</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
+        <v>682</v>
+      </c>
+      <c r="N21" t="s">
+        <v>769</v>
+      </c>
+      <c r="O21" t="s">
+        <v>702</v>
+      </c>
+      <c r="P21" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>704</v>
+      </c>
+      <c r="R21" t="s">
+        <v>701</v>
+      </c>
+      <c r="S21" t="s">
         <v>762</v>
       </c>
-      <c r="M21" t="s">
-        <v>683</v>
-      </c>
-      <c r="N21" t="s">
-        <v>770</v>
-      </c>
-      <c r="O21" t="s">
-        <v>703</v>
-      </c>
-      <c r="P21" t="s">
-        <v>704</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>705</v>
-      </c>
-      <c r="R21" t="s">
-        <v>702</v>
-      </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>763</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>764</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>765</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
+        <v>696</v>
+      </c>
+      <c r="X21" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>776</v>
+      </c>
+      <c r="Z21" t="s">
         <v>766</v>
-      </c>
-      <c r="W21" t="s">
-        <v>697</v>
-      </c>
-      <c r="X21" t="s">
-        <v>696</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>777</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B22" t="s">
         <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D22" t="s">
         <v>131</v>
@@ -6408,81 +6432,81 @@
         <v>142</v>
       </c>
       <c r="F22" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G22" t="s">
         <v>143</v>
       </c>
       <c r="H22" t="s">
+        <v>698</v>
+      </c>
+      <c r="I22" t="s">
         <v>699</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>759</v>
+      </c>
+      <c r="K22" t="s">
+        <v>760</v>
+      </c>
+      <c r="L22" t="s">
+        <v>761</v>
+      </c>
+      <c r="M22" t="s">
         <v>700</v>
       </c>
-      <c r="J22" t="s">
-        <v>760</v>
-      </c>
-      <c r="K22" t="s">
-        <v>761</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
+        <v>682</v>
+      </c>
+      <c r="O22" t="s">
+        <v>769</v>
+      </c>
+      <c r="P22" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>703</v>
+      </c>
+      <c r="R22" t="s">
+        <v>704</v>
+      </c>
+      <c r="S22" t="s">
+        <v>701</v>
+      </c>
+      <c r="T22" t="s">
         <v>762</v>
       </c>
-      <c r="M22" t="s">
-        <v>701</v>
-      </c>
-      <c r="N22" t="s">
-        <v>683</v>
-      </c>
-      <c r="O22" t="s">
-        <v>770</v>
-      </c>
-      <c r="P22" t="s">
-        <v>703</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>704</v>
-      </c>
-      <c r="R22" t="s">
-        <v>705</v>
-      </c>
-      <c r="S22" t="s">
-        <v>702</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>763</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>764</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
         <v>765</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
+        <v>696</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>695</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>776</v>
+      </c>
+      <c r="AA22" t="s">
         <v>766</v>
-      </c>
-      <c r="X22" t="s">
-        <v>697</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>696</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>777</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B23" t="s">
         <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D23" t="s">
         <v>131</v>
@@ -6491,87 +6515,87 @@
         <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G23" t="s">
         <v>143</v>
       </c>
       <c r="H23" t="s">
+        <v>698</v>
+      </c>
+      <c r="I23" t="s">
         <v>699</v>
       </c>
-      <c r="I23" t="s">
-        <v>700</v>
-      </c>
       <c r="J23" t="s">
+        <v>759</v>
+      </c>
+      <c r="K23" t="s">
         <v>760</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>761</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
+        <v>704</v>
+      </c>
+      <c r="N23" t="s">
+        <v>701</v>
+      </c>
+      <c r="O23" t="s">
+        <v>770</v>
+      </c>
+      <c r="P23" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>771</v>
+      </c>
+      <c r="R23" t="s">
+        <v>772</v>
+      </c>
+      <c r="S23" t="s">
+        <v>773</v>
+      </c>
+      <c r="T23" t="s">
+        <v>774</v>
+      </c>
+      <c r="U23" t="s">
+        <v>775</v>
+      </c>
+      <c r="V23" t="s">
         <v>762</v>
       </c>
-      <c r="M23" t="s">
-        <v>705</v>
-      </c>
-      <c r="N23" t="s">
-        <v>702</v>
-      </c>
-      <c r="O23" t="s">
-        <v>771</v>
-      </c>
-      <c r="P23" t="s">
-        <v>706</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>772</v>
-      </c>
-      <c r="R23" t="s">
-        <v>773</v>
-      </c>
-      <c r="S23" t="s">
-        <v>774</v>
-      </c>
-      <c r="T23" t="s">
-        <v>775</v>
-      </c>
-      <c r="U23" t="s">
+      <c r="W23" t="s">
+        <v>763</v>
+      </c>
+      <c r="X23" t="s">
+        <v>764</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>696</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>695</v>
+      </c>
+      <c r="AB23" t="s">
         <v>776</v>
       </c>
-      <c r="V23" t="s">
-        <v>763</v>
-      </c>
-      <c r="W23" t="s">
-        <v>764</v>
-      </c>
-      <c r="X23" t="s">
-        <v>765</v>
-      </c>
-      <c r="Y23" t="s">
+      <c r="AC23" t="s">
         <v>766</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>697</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>696</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>777</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B24" t="s">
         <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D24" t="s">
         <v>131</v>
@@ -6580,87 +6604,87 @@
         <v>142</v>
       </c>
       <c r="F24" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G24" t="s">
         <v>143</v>
       </c>
       <c r="H24" t="s">
+        <v>698</v>
+      </c>
+      <c r="I24" t="s">
         <v>699</v>
       </c>
-      <c r="I24" t="s">
-        <v>700</v>
-      </c>
       <c r="J24" t="s">
+        <v>759</v>
+      </c>
+      <c r="K24" t="s">
         <v>760</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>761</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
+        <v>704</v>
+      </c>
+      <c r="N24" t="s">
+        <v>701</v>
+      </c>
+      <c r="O24" t="s">
+        <v>770</v>
+      </c>
+      <c r="P24" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>771</v>
+      </c>
+      <c r="R24" t="s">
+        <v>772</v>
+      </c>
+      <c r="S24" t="s">
+        <v>773</v>
+      </c>
+      <c r="T24" t="s">
+        <v>774</v>
+      </c>
+      <c r="U24" t="s">
+        <v>775</v>
+      </c>
+      <c r="V24" t="s">
         <v>762</v>
       </c>
-      <c r="M24" t="s">
-        <v>705</v>
-      </c>
-      <c r="N24" t="s">
-        <v>702</v>
-      </c>
-      <c r="O24" t="s">
-        <v>771</v>
-      </c>
-      <c r="P24" t="s">
-        <v>706</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>772</v>
-      </c>
-      <c r="R24" t="s">
-        <v>773</v>
-      </c>
-      <c r="S24" t="s">
-        <v>774</v>
-      </c>
-      <c r="T24" t="s">
-        <v>775</v>
-      </c>
-      <c r="U24" t="s">
+      <c r="W24" t="s">
+        <v>763</v>
+      </c>
+      <c r="X24" t="s">
+        <v>764</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>696</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>695</v>
+      </c>
+      <c r="AB24" t="s">
         <v>776</v>
       </c>
-      <c r="V24" t="s">
-        <v>763</v>
-      </c>
-      <c r="W24" t="s">
-        <v>764</v>
-      </c>
-      <c r="X24" t="s">
-        <v>765</v>
-      </c>
-      <c r="Y24" t="s">
+      <c r="AC24" t="s">
         <v>766</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>697</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>696</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>777</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B25" t="s">
         <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D25" t="s">
         <v>131</v>
@@ -6669,43 +6693,43 @@
         <v>142</v>
       </c>
       <c r="F25" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G25" t="s">
         <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I25" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K25" t="s">
+        <v>762</v>
+      </c>
+      <c r="L25" t="s">
         <v>763</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>764</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>765</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
+        <v>696</v>
+      </c>
+      <c r="P25" t="s">
+        <v>695</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>776</v>
+      </c>
+      <c r="R25" t="s">
         <v>766</v>
-      </c>
-      <c r="O25" t="s">
-        <v>697</v>
-      </c>
-      <c r="P25" t="s">
-        <v>696</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>777</v>
-      </c>
-      <c r="R25" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.35">
@@ -6725,19 +6749,19 @@
         <v>137</v>
       </c>
       <c r="F26" t="s">
+        <v>666</v>
+      </c>
+      <c r="G26" t="s">
+        <v>663</v>
+      </c>
+      <c r="H26" t="s">
+        <v>650</v>
+      </c>
+      <c r="I26" t="s">
+        <v>651</v>
+      </c>
+      <c r="J26" t="s">
         <v>667</v>
-      </c>
-      <c r="G26" t="s">
-        <v>664</v>
-      </c>
-      <c r="H26" t="s">
-        <v>651</v>
-      </c>
-      <c r="I26" t="s">
-        <v>652</v>
-      </c>
-      <c r="J26" t="s">
-        <v>668</v>
       </c>
       <c r="K26" t="s">
         <v>636</v>
@@ -7608,7 +7632,7 @@
     </row>
     <row r="13" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>109</v>
@@ -7723,7 +7747,7 @@
     </row>
     <row r="14" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>109</v>
@@ -7852,7 +7876,7 @@
     </row>
     <row r="15" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>109</v>
@@ -7981,7 +8005,7 @@
     </row>
     <row r="16" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>109</v>
@@ -8102,7 +8126,7 @@
     </row>
     <row r="17" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>109</v>
@@ -8223,7 +8247,7 @@
     </row>
     <row r="18" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>109</v>
@@ -8344,7 +8368,7 @@
     </row>
     <row r="19" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>109</v>
@@ -8465,7 +8489,7 @@
     </row>
     <row r="20" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>109</v>
@@ -8586,7 +8610,7 @@
     </row>
     <row r="21" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>109</v>
@@ -8717,7 +8741,7 @@
     </row>
     <row r="22" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>109</v>
@@ -8851,7 +8875,7 @@
     </row>
     <row r="23" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>109</v>
@@ -8986,7 +9010,7 @@
     </row>
     <row r="24" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>109</v>
@@ -9121,7 +9145,7 @@
     </row>
     <row r="25" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>109</v>
@@ -10226,7 +10250,7 @@
   </sheetPr>
   <dimension ref="A1:CK85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -10619,7 +10643,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -10726,7 +10750,7 @@
     </row>
     <row r="12" spans="1:89" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -10738,7 +10762,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -10747,7 +10771,7 @@
         <v>91</v>
       </c>
       <c r="H12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I12" t="s">
         <v>624</v>
@@ -10785,7 +10809,7 @@
     </row>
     <row r="13" spans="1:89" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -10806,7 +10830,7 @@
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I13" t="s">
         <v>14</v>
@@ -10815,7 +10839,7 @@
         <v>91</v>
       </c>
       <c r="K13" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L13" t="s">
         <v>624</v>
@@ -10865,7 +10889,7 @@
     </row>
     <row r="14" spans="1:89" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -10883,7 +10907,7 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
@@ -10892,7 +10916,7 @@
         <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K14" t="s">
         <v>624</v>
@@ -10933,7 +10957,7 @@
     </row>
     <row r="15" spans="1:89" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -10951,7 +10975,7 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H15" t="s">
         <v>14</v>
@@ -10960,7 +10984,7 @@
         <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K15" t="s">
         <v>624</v>
@@ -11013,7 +11037,7 @@
     </row>
     <row r="16" spans="1:89" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -11031,7 +11055,7 @@
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
@@ -11040,7 +11064,7 @@
         <v>91</v>
       </c>
       <c r="J16" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K16" t="s">
         <v>624</v>
@@ -11096,7 +11120,7 @@
     </row>
     <row r="17" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -11114,7 +11138,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -11123,7 +11147,7 @@
         <v>91</v>
       </c>
       <c r="J17" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K17" t="s">
         <v>624</v>
@@ -11164,7 +11188,7 @@
     </row>
     <row r="18" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -11182,7 +11206,7 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -11191,7 +11215,7 @@
         <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K18" t="s">
         <v>624</v>
@@ -11232,7 +11256,7 @@
     </row>
     <row r="19" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -11250,7 +11274,7 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -11259,7 +11283,7 @@
         <v>91</v>
       </c>
       <c r="J19" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K19" t="s">
         <v>624</v>
@@ -11300,7 +11324,7 @@
     </row>
     <row r="20" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -11318,7 +11342,7 @@
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -11327,7 +11351,7 @@
         <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K20" t="s">
         <v>624</v>
@@ -11368,7 +11392,7 @@
     </row>
     <row r="21" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -11386,7 +11410,7 @@
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
@@ -11395,7 +11419,7 @@
         <v>91</v>
       </c>
       <c r="J21" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K21" t="s">
         <v>624</v>
@@ -11457,7 +11481,7 @@
     </row>
     <row r="22" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -11475,7 +11499,7 @@
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -11484,7 +11508,7 @@
         <v>91</v>
       </c>
       <c r="J22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K22" t="s">
         <v>624</v>
@@ -11546,7 +11570,7 @@
     </row>
     <row r="23" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -11564,10 +11588,10 @@
         <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I23" t="s">
         <v>14</v>
@@ -11576,7 +11600,7 @@
         <v>91</v>
       </c>
       <c r="K23" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L23" t="s">
         <v>624</v>
@@ -11626,7 +11650,7 @@
     </row>
     <row r="24" spans="1:29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -11644,10 +11668,10 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H24" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I24" t="s">
         <v>14</v>
@@ -12014,7 +12038,7 @@
         <v>553</v>
       </c>
       <c r="B50" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="51" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
@@ -12199,7 +12223,7 @@
         <v>555</v>
       </c>
       <c r="B72" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="73" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
@@ -12292,7 +12316,7 @@
         <v>558</v>
       </c>
       <c r="B81" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="82" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
@@ -12300,7 +12324,7 @@
         <v>560</v>
       </c>
       <c r="B82" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="83" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
@@ -12327,40 +12351,40 @@
         <v>11</v>
       </c>
       <c r="C85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="J85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="L85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="M85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="N85" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -12381,8 +12405,8 @@
   </sheetPr>
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12632,7 +12656,7 @@
         <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="I5" t="s">
         <v>210</v>
@@ -12693,13 +12717,13 @@
         <v>191</v>
       </c>
       <c r="F7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G7" t="s">
         <v>604</v>
       </c>
       <c r="H7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -12713,7 +12737,7 @@
         <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
@@ -12777,7 +12801,7 @@
         <v>604</v>
       </c>
       <c r="G10" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
@@ -12791,7 +12815,7 @@
         <v>623</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E11" t="s">
         <v>192</v>
@@ -12821,10 +12845,10 @@
         <v>639</v>
       </c>
       <c r="N11" t="s">
+        <v>657</v>
+      </c>
+      <c r="O11" t="s">
         <v>658</v>
-      </c>
-      <c r="O11" t="s">
-        <v>659</v>
       </c>
       <c r="P11" t="s">
         <v>640</v>
@@ -12850,15 +12874,15 @@
         <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B13" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C13" t="s">
         <v>623</v>
@@ -12879,13 +12903,13 @@
         <v>222</v>
       </c>
       <c r="I13" t="s">
+        <v>679</v>
+      </c>
+      <c r="J13" t="s">
         <v>680</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>681</v>
-      </c>
-      <c r="K13" t="s">
-        <v>682</v>
       </c>
       <c r="L13" t="s">
         <v>225</v>
@@ -12903,24 +12927,24 @@
         <v>229</v>
       </c>
       <c r="Q13" t="s">
+        <v>689</v>
+      </c>
+      <c r="R13" t="s">
         <v>690</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>691</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>692</v>
-      </c>
-      <c r="T13" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B14" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C14" t="s">
         <v>623</v>
@@ -12950,22 +12974,22 @@
         <v>222</v>
       </c>
       <c r="L14" t="s">
+        <v>679</v>
+      </c>
+      <c r="M14" t="s">
         <v>680</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>681</v>
-      </c>
-      <c r="N14" t="s">
-        <v>682</v>
       </c>
       <c r="O14" t="s">
         <v>224</v>
       </c>
       <c r="P14" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q14" t="s">
         <v>688</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>689</v>
       </c>
       <c r="R14" t="s">
         <v>225</v>
@@ -12986,24 +13010,24 @@
         <v>229</v>
       </c>
       <c r="X14" t="s">
+        <v>689</v>
+      </c>
+      <c r="Y14" t="s">
         <v>690</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>691</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>692</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B15" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C15" t="s">
         <v>623</v>
@@ -13033,22 +13057,22 @@
         <v>222</v>
       </c>
       <c r="L15" t="s">
+        <v>679</v>
+      </c>
+      <c r="M15" t="s">
         <v>680</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>681</v>
-      </c>
-      <c r="N15" t="s">
-        <v>682</v>
       </c>
       <c r="O15" t="s">
         <v>224</v>
       </c>
       <c r="P15" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q15" t="s">
         <v>688</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>689</v>
       </c>
       <c r="R15" t="s">
         <v>225</v>
@@ -13069,24 +13093,24 @@
         <v>229</v>
       </c>
       <c r="X15" t="s">
+        <v>689</v>
+      </c>
+      <c r="Y15" t="s">
         <v>690</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>691</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>692</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B16" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C16" t="s">
         <v>623</v>
@@ -13113,16 +13137,16 @@
         <v>222</v>
       </c>
       <c r="K16" t="s">
+        <v>679</v>
+      </c>
+      <c r="L16" t="s">
         <v>680</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>681</v>
       </c>
-      <c r="M16" t="s">
-        <v>682</v>
-      </c>
       <c r="N16" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O16" t="s">
         <v>225</v>
@@ -13140,24 +13164,24 @@
         <v>229</v>
       </c>
       <c r="T16" t="s">
+        <v>689</v>
+      </c>
+      <c r="U16" t="s">
         <v>690</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>691</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>692</v>
-      </c>
-      <c r="W16" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B17" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C17" t="s">
         <v>623</v>
@@ -13184,16 +13208,16 @@
         <v>222</v>
       </c>
       <c r="K17" t="s">
+        <v>679</v>
+      </c>
+      <c r="L17" t="s">
         <v>680</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>681</v>
       </c>
-      <c r="M17" t="s">
-        <v>682</v>
-      </c>
       <c r="N17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O17" t="s">
         <v>225</v>
@@ -13211,24 +13235,24 @@
         <v>229</v>
       </c>
       <c r="T17" t="s">
+        <v>689</v>
+      </c>
+      <c r="U17" t="s">
         <v>690</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>691</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>692</v>
-      </c>
-      <c r="W17" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B18" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C18" t="s">
         <v>623</v>
@@ -13255,16 +13279,16 @@
         <v>222</v>
       </c>
       <c r="K18" t="s">
+        <v>679</v>
+      </c>
+      <c r="L18" t="s">
         <v>680</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>681</v>
       </c>
-      <c r="M18" t="s">
-        <v>682</v>
-      </c>
       <c r="N18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O18" t="s">
         <v>225</v>
@@ -13282,24 +13306,24 @@
         <v>229</v>
       </c>
       <c r="T18" t="s">
+        <v>689</v>
+      </c>
+      <c r="U18" t="s">
         <v>690</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>691</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>692</v>
-      </c>
-      <c r="W18" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C19" t="s">
         <v>623</v>
@@ -13326,16 +13350,16 @@
         <v>222</v>
       </c>
       <c r="K19" t="s">
+        <v>679</v>
+      </c>
+      <c r="L19" t="s">
         <v>680</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>681</v>
       </c>
-      <c r="M19" t="s">
-        <v>682</v>
-      </c>
       <c r="N19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O19" t="s">
         <v>225</v>
@@ -13353,24 +13377,24 @@
         <v>229</v>
       </c>
       <c r="T19" t="s">
+        <v>689</v>
+      </c>
+      <c r="U19" t="s">
         <v>690</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>691</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>692</v>
-      </c>
-      <c r="W19" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>735</v>
+      </c>
+      <c r="B20" t="s">
         <v>736</v>
-      </c>
-      <c r="B20" t="s">
-        <v>737</v>
       </c>
       <c r="C20" t="s">
         <v>623</v>
@@ -13397,16 +13421,16 @@
         <v>222</v>
       </c>
       <c r="K20" t="s">
+        <v>679</v>
+      </c>
+      <c r="L20" t="s">
         <v>680</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>681</v>
       </c>
-      <c r="M20" t="s">
-        <v>682</v>
-      </c>
       <c r="N20" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O20" t="s">
         <v>225</v>
@@ -13424,24 +13448,24 @@
         <v>229</v>
       </c>
       <c r="T20" t="s">
+        <v>689</v>
+      </c>
+      <c r="U20" t="s">
         <v>690</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>691</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>692</v>
-      </c>
-      <c r="W20" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>739</v>
+      </c>
+      <c r="B21" t="s">
         <v>740</v>
-      </c>
-      <c r="B21" t="s">
-        <v>741</v>
       </c>
       <c r="C21" t="s">
         <v>623</v>
@@ -13468,28 +13492,28 @@
         <v>222</v>
       </c>
       <c r="K21" t="s">
+        <v>679</v>
+      </c>
+      <c r="L21" t="s">
         <v>680</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>681</v>
-      </c>
-      <c r="M21" t="s">
-        <v>682</v>
       </c>
       <c r="N21" t="s">
         <v>235</v>
       </c>
       <c r="O21" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="P21" t="s">
         <v>236</v>
       </c>
       <c r="Q21" t="s">
+        <v>684</v>
+      </c>
+      <c r="R21" t="s">
         <v>685</v>
-      </c>
-      <c r="R21" t="s">
-        <v>686</v>
       </c>
       <c r="S21" t="s">
         <v>225</v>
@@ -13507,24 +13531,24 @@
         <v>229</v>
       </c>
       <c r="X21" t="s">
+        <v>689</v>
+      </c>
+      <c r="Y21" t="s">
         <v>690</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>691</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AA21" t="s">
         <v>692</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B22" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C22" t="s">
         <v>623</v>
@@ -13551,13 +13575,13 @@
         <v>222</v>
       </c>
       <c r="K22" t="s">
+        <v>679</v>
+      </c>
+      <c r="L22" t="s">
         <v>680</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>681</v>
-      </c>
-      <c r="M22" t="s">
-        <v>682</v>
       </c>
       <c r="N22" t="s">
         <v>224</v>
@@ -13566,16 +13590,16 @@
         <v>235</v>
       </c>
       <c r="P22" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Q22" t="s">
         <v>236</v>
       </c>
       <c r="R22" t="s">
+        <v>684</v>
+      </c>
+      <c r="S22" t="s">
         <v>685</v>
-      </c>
-      <c r="S22" t="s">
-        <v>686</v>
       </c>
       <c r="T22" t="s">
         <v>225</v>
@@ -13593,24 +13617,24 @@
         <v>229</v>
       </c>
       <c r="Y22" t="s">
+        <v>689</v>
+      </c>
+      <c r="Z22" t="s">
         <v>690</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>691</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>692</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B23" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C23" t="s">
         <v>623</v>
@@ -13637,16 +13661,16 @@
         <v>222</v>
       </c>
       <c r="K23" t="s">
+        <v>679</v>
+      </c>
+      <c r="L23" t="s">
         <v>680</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>681</v>
       </c>
-      <c r="M23" t="s">
-        <v>682</v>
-      </c>
       <c r="N23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O23" t="s">
         <v>225</v>
@@ -13658,7 +13682,7 @@
         <v>238</v>
       </c>
       <c r="R23" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S23" t="s">
         <v>231</v>
@@ -13685,24 +13709,24 @@
         <v>229</v>
       </c>
       <c r="AA23" t="s">
+        <v>689</v>
+      </c>
+      <c r="AB23" t="s">
         <v>690</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AC23" t="s">
         <v>691</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AD23" t="s">
         <v>692</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B24" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C24" t="s">
         <v>623</v>
@@ -13729,16 +13753,16 @@
         <v>222</v>
       </c>
       <c r="K24" t="s">
+        <v>679</v>
+      </c>
+      <c r="L24" t="s">
         <v>680</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>681</v>
       </c>
-      <c r="M24" t="s">
-        <v>682</v>
-      </c>
       <c r="N24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O24" t="s">
         <v>225</v>
@@ -13750,7 +13774,7 @@
         <v>238</v>
       </c>
       <c r="R24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S24" t="s">
         <v>231</v>
@@ -13777,24 +13801,24 @@
         <v>229</v>
       </c>
       <c r="AA24" t="s">
+        <v>689</v>
+      </c>
+      <c r="AB24" t="s">
         <v>690</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AC24" t="s">
         <v>691</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AD24" t="s">
         <v>692</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B25" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C25" t="s">
         <v>623</v>
@@ -13836,16 +13860,16 @@
         <v>229</v>
       </c>
       <c r="P25" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q25" t="s">
         <v>690</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>691</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>692</v>
-      </c>
-      <c r="S25" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.35">
@@ -13868,10 +13892,10 @@
         <v>193</v>
       </c>
       <c r="G26" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H26" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I26" t="s">
         <v>212</v>
@@ -13880,7 +13904,7 @@
         <v>213</v>
       </c>
       <c r="K26" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="L26" t="s">
         <v>638</v>
@@ -14101,46 +14125,46 @@
         <v>127</v>
       </c>
       <c r="B39" t="s">
+        <v>788</v>
+      </c>
+      <c r="C39" t="s">
         <v>789</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>790</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>791</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>792</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>793</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>794</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>795</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>796</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>797</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>798</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>799</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>800</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>801</v>
-      </c>
-      <c r="O39" t="s">
-        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -14206,19 +14230,19 @@
         <v>127</v>
       </c>
       <c r="B2" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2" t="s">
         <v>784</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>785</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>786</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>787</v>
-      </c>
-      <c r="F2" t="s">
-        <v>788</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -14406,13 +14430,13 @@
         <v>463</v>
       </c>
       <c r="B10" t="s">
+        <v>780</v>
+      </c>
+      <c r="C10" t="s">
         <v>781</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>782</v>
-      </c>
-      <c r="D10" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -14420,13 +14444,13 @@
         <v>466</v>
       </c>
       <c r="B11" t="s">
+        <v>780</v>
+      </c>
+      <c r="C11" t="s">
         <v>781</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>782</v>
-      </c>
-      <c r="D11" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -14434,13 +14458,13 @@
         <v>460</v>
       </c>
       <c r="B12" t="s">
+        <v>780</v>
+      </c>
+      <c r="C12" t="s">
         <v>781</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>782</v>
-      </c>
-      <c r="D12" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -14448,13 +14472,13 @@
         <v>468</v>
       </c>
       <c r="B13" t="s">
+        <v>780</v>
+      </c>
+      <c r="C13" t="s">
         <v>781</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>782</v>
-      </c>
-      <c r="D13" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
@@ -14462,13 +14486,13 @@
         <v>471</v>
       </c>
       <c r="B14" t="s">
+        <v>780</v>
+      </c>
+      <c r="C14" t="s">
         <v>781</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>782</v>
-      </c>
-      <c r="D14" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -14476,13 +14500,13 @@
         <v>467</v>
       </c>
       <c r="B15" t="s">
+        <v>780</v>
+      </c>
+      <c r="C15" t="s">
         <v>781</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>782</v>
-      </c>
-      <c r="D15" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -14490,13 +14514,13 @@
         <v>461</v>
       </c>
       <c r="B16" t="s">
+        <v>780</v>
+      </c>
+      <c r="C16" t="s">
         <v>781</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>782</v>
-      </c>
-      <c r="D16" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -14504,13 +14528,13 @@
         <v>462</v>
       </c>
       <c r="B17" t="s">
+        <v>780</v>
+      </c>
+      <c r="C17" t="s">
         <v>781</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>782</v>
-      </c>
-      <c r="D17" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -14518,13 +14542,13 @@
         <v>469</v>
       </c>
       <c r="B18" t="s">
+        <v>780</v>
+      </c>
+      <c r="C18" t="s">
         <v>781</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>782</v>
-      </c>
-      <c r="D18" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -14532,13 +14556,13 @@
         <v>470</v>
       </c>
       <c r="B19" t="s">
+        <v>780</v>
+      </c>
+      <c r="C19" t="s">
         <v>781</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>782</v>
-      </c>
-      <c r="D19" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -14546,13 +14570,13 @@
         <v>465</v>
       </c>
       <c r="B20" t="s">
+        <v>780</v>
+      </c>
+      <c r="C20" t="s">
         <v>781</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>782</v>
-      </c>
-      <c r="D20" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -14560,13 +14584,13 @@
         <v>472</v>
       </c>
       <c r="B21" t="s">
+        <v>780</v>
+      </c>
+      <c r="C21" t="s">
         <v>781</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>782</v>
-      </c>
-      <c r="D21" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -14574,13 +14598,13 @@
         <v>459</v>
       </c>
       <c r="B22" t="s">
+        <v>780</v>
+      </c>
+      <c r="C22" t="s">
         <v>781</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>782</v>
-      </c>
-      <c r="D22" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -14588,13 +14612,13 @@
         <v>464</v>
       </c>
       <c r="B23" t="s">
+        <v>780</v>
+      </c>
+      <c r="C23" t="s">
         <v>781</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>782</v>
-      </c>
-      <c r="D23" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add operational limit conditions to core to allow modification in the installation interface
</commit_message>
<xml_diff>
--- a/dds/installation.xlsx
+++ b/dds/installation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="590" yWindow="1010" windowWidth="10210" windowHeight="6080" tabRatio="474" activeTab="3"/>
+    <workbookView xWindow="590" yWindow="1010" windowWidth="10210" windowHeight="6080" tabRatio="474" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3231" uniqueCount="870">
   <si>
     <t>Identifier</t>
   </si>
@@ -2462,6 +2462,186 @@
   </si>
   <si>
     <t>degrees</t>
+  </si>
+  <si>
+    <t>Wave Height Operational Limits</t>
+  </si>
+  <si>
+    <t>SimpleDictColumn</t>
+  </si>
+  <si>
+    <t>Per operation limit conditions for significant wave height</t>
+  </si>
+  <si>
+    <t>Hs Limit</t>
+  </si>
+  <si>
+    <t>reference.view_operations_limit_hs</t>
+  </si>
+  <si>
+    <t>component.operations_limit_hs</t>
+  </si>
+  <si>
+    <t>operations_type</t>
+  </si>
+  <si>
+    <t>hs_limit</t>
+  </si>
+  <si>
+    <t>Vessel Positioning + Connection to cable pull-head + Cable float-out + Cable lay into pre-excavated trench</t>
+  </si>
+  <si>
+    <t>Vessel positioning + Connection to cable pull-head + Cable float-out + Cable pull-in through HDD conduit</t>
+  </si>
+  <si>
+    <t>Deploy of Cable Burial Tool</t>
+  </si>
+  <si>
+    <t>Recover cable burial tool</t>
+  </si>
+  <si>
+    <t>Cable lay and burial through cable route</t>
+  </si>
+  <si>
+    <t>Cable lay through cable route</t>
+  </si>
+  <si>
+    <t>Cable lay through open trench</t>
+  </si>
+  <si>
+    <t>Cable lay with split pipes</t>
+  </si>
+  <si>
+    <t>Cable lay with buoyancy modules</t>
+  </si>
+  <si>
+    <t>Conduct dry-mate connection on deck</t>
+  </si>
+  <si>
+    <t>Conduct splice connection on deck</t>
+  </si>
+  <si>
+    <t>Connect to guide wire + Lower cable and connection equip + Perform wet-mate connect + Recover connection equip</t>
+  </si>
+  <si>
+    <t>J-tube entrance inspection + Guide wire connection + Cable lay + Cable pull + Cable connection</t>
+  </si>
+  <si>
+    <t>Lower cable-end to the seabed</t>
+  </si>
+  <si>
+    <t>Lift cable-end from seabed</t>
+  </si>
+  <si>
+    <t>Lower collection point to the seabed</t>
+  </si>
+  <si>
+    <t>Lift top-side platform</t>
+  </si>
+  <si>
+    <t>Connect top-side platform to the support structure</t>
+  </si>
+  <si>
+    <t>Lift and overboard concrete mattress + Lower concrete mattress to seabed + Position and release concrete mattress + Recover installation frame</t>
+  </si>
+  <si>
+    <t>Lift and overboard rock filter bag + Lower rock filter bag to seabed + Position and release concrete mattress</t>
+  </si>
+  <si>
+    <t>Wave Period Operational Limits</t>
+  </si>
+  <si>
+    <t>Per operation limit conditions for peak wave period</t>
+  </si>
+  <si>
+    <t>component.operations_limit_tp</t>
+  </si>
+  <si>
+    <t>component.operations_limit_ws</t>
+  </si>
+  <si>
+    <t>Wind Speed Operational Limits</t>
+  </si>
+  <si>
+    <t>component.operations_limit_cs</t>
+  </si>
+  <si>
+    <t>Current Speed Operational Limits</t>
+  </si>
+  <si>
+    <t>Per operation limit conditions for current speed</t>
+  </si>
+  <si>
+    <t>Per operation limit conditions for wind speed</t>
+  </si>
+  <si>
+    <t>Tp Limit</t>
+  </si>
+  <si>
+    <t>Wind Velocity Limit</t>
+  </si>
+  <si>
+    <t>Current Velocity Limit</t>
+  </si>
+  <si>
+    <t>reference.view_operations_limit_tp</t>
+  </si>
+  <si>
+    <t>reference.view_operations_limit_ws</t>
+  </si>
+  <si>
+    <t>reference.view_operations_limit_cs</t>
+  </si>
+  <si>
+    <t>tp_limit</t>
+  </si>
+  <si>
+    <t>ws_limit</t>
+  </si>
+  <si>
+    <t>cs_limit</t>
+  </si>
+  <si>
+    <t>Seafloor &amp; equipment preparation</t>
+  </si>
+  <si>
+    <t>Grouting</t>
+  </si>
+  <si>
+    <t>Grouting equipment removal</t>
+  </si>
+  <si>
+    <t>Guiding template positioning + seafloor preparation equipment preparation</t>
+  </si>
+  <si>
+    <t>Seafloor preparation + support structure positioning and equipment preparation</t>
+  </si>
+  <si>
+    <t>Driven pile foundation or anchor seafloor penetration through drilling rig + positioning</t>
+  </si>
+  <si>
+    <t>Driven pile foundation or anchor seafloor penetration through hammering + positioning</t>
+  </si>
+  <si>
+    <t>Driven pile foundation or anchor seafloor penetration through vibro-driving + positioning</t>
+  </si>
+  <si>
+    <t>Gravity based foundation or anchor lowering</t>
+  </si>
+  <si>
+    <t>Lowering mooring lines + Drag-embedment anchor seafloor penetration + Tensioning</t>
+  </si>
+  <si>
+    <t>Lowering mooring lines + Connecting end of mooring line to pre-installed pile + Tensioning</t>
+  </si>
+  <si>
+    <t>Lowering anchors with mooring lines + Direct-embedment anchor seafloor penetration through suction-embedment + Tensioning</t>
+  </si>
+  <si>
+    <t>Lowering anchors with mooring lines + Direct-embedment anchor seafloor penetration through jetting-embedment + Tensioning</t>
+  </si>
+  <si>
+    <t>Lowering anchors with mooring lines + Direct-embedment anchor seafloor penetration through mechanical-embedment + Tensioning</t>
   </si>
 </sst>
 </file>
@@ -3162,11 +3342,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5242,6 +5422,62 @@
       <c r="G119" s="30"/>
       <c r="H119" s="30"/>
     </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B120" s="28" t="s">
+        <v>811</v>
+      </c>
+      <c r="C120" s="47" t="s">
+        <v>810</v>
+      </c>
+      <c r="D120" s="47" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B121" s="28" t="s">
+        <v>811</v>
+      </c>
+      <c r="C121" s="47" t="s">
+        <v>838</v>
+      </c>
+      <c r="D121" s="47" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B122" s="28" t="s">
+        <v>811</v>
+      </c>
+      <c r="C122" s="47" t="s">
+        <v>842</v>
+      </c>
+      <c r="D122" s="47" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B123" s="28" t="s">
+        <v>811</v>
+      </c>
+      <c r="C123" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="D123" s="47" t="s">
+        <v>845</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H119">
     <sortState ref="A2:H119">
@@ -5261,11 +5497,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A47" sqref="A47"/>
+      <selection pane="topRight" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7126,6 +7362,50 @@
         <v>808</v>
       </c>
     </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" t="s">
+        <v>849</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE1">
     <sortState ref="A2:AE44">
@@ -7142,10 +7422,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:CK102"/>
+  <dimension ref="A1:CK106"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD72"/>
+    <sheetView topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10296,6 +10576,38 @@
         <v>110</v>
       </c>
     </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE1"/>
   <sortState ref="A1:Z58">
@@ -10311,10 +10623,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:CK86"/>
+  <dimension ref="A1:CK90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12461,6 +12773,38 @@
         <v>809</v>
       </c>
     </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A87" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A88" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A89" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A90" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE1">
     <sortState ref="A2:AE84">
@@ -12477,10 +12821,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AD39"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14241,6 +14585,62 @@
         <v>799</v>
       </c>
     </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B40" t="s">
+        <v>814</v>
+      </c>
+      <c r="C40" t="s">
+        <v>816</v>
+      </c>
+      <c r="D40" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B41" t="s">
+        <v>850</v>
+      </c>
+      <c r="C41" t="s">
+        <v>816</v>
+      </c>
+      <c r="D41" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B42" t="s">
+        <v>851</v>
+      </c>
+      <c r="C42" t="s">
+        <v>816</v>
+      </c>
+      <c r="D42" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A43" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B43" t="s">
+        <v>852</v>
+      </c>
+      <c r="C43" t="s">
+        <v>816</v>
+      </c>
+      <c r="D43" t="s">
+        <v>855</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:BX38">
     <sortState ref="A2:BX26">
@@ -14257,10 +14657,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14597,7 +14997,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>460</v>
       </c>
@@ -14611,7 +15011,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>467</v>
       </c>
@@ -14625,7 +15025,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>468</v>
       </c>
@@ -14639,7 +15039,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>463</v>
       </c>
@@ -14653,7 +15053,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>470</v>
       </c>
@@ -14667,7 +15067,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>457</v>
       </c>
@@ -14681,7 +15081,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>462</v>
       </c>
@@ -14695,7 +15095,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>561</v>
       </c>
@@ -14706,7 +15106,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>554</v>
       </c>
@@ -14726,7 +15126,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>555</v>
       </c>
@@ -14737,7 +15137,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>557</v>
       </c>
@@ -14748,7 +15148,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>559</v>
       </c>
@@ -14786,7 +15186,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>560</v>
       </c>
@@ -14798,6 +15198,386 @@
       </c>
       <c r="D29" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A30" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="B30" t="s">
+        <v>818</v>
+      </c>
+      <c r="C30" t="s">
+        <v>819</v>
+      </c>
+      <c r="D30" t="s">
+        <v>820</v>
+      </c>
+      <c r="E30" t="s">
+        <v>821</v>
+      </c>
+      <c r="F30" t="s">
+        <v>822</v>
+      </c>
+      <c r="G30" t="s">
+        <v>823</v>
+      </c>
+      <c r="H30" t="s">
+        <v>824</v>
+      </c>
+      <c r="I30" t="s">
+        <v>825</v>
+      </c>
+      <c r="J30" t="s">
+        <v>826</v>
+      </c>
+      <c r="K30" t="s">
+        <v>827</v>
+      </c>
+      <c r="L30" t="s">
+        <v>828</v>
+      </c>
+      <c r="M30" t="s">
+        <v>829</v>
+      </c>
+      <c r="N30" t="s">
+        <v>830</v>
+      </c>
+      <c r="O30" t="s">
+        <v>831</v>
+      </c>
+      <c r="P30" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>833</v>
+      </c>
+      <c r="R30" t="s">
+        <v>834</v>
+      </c>
+      <c r="S30" t="s">
+        <v>835</v>
+      </c>
+      <c r="T30" t="s">
+        <v>836</v>
+      </c>
+      <c r="U30" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A31" s="14" t="s">
+        <v>840</v>
+      </c>
+      <c r="B31" t="s">
+        <v>856</v>
+      </c>
+      <c r="C31" t="s">
+        <v>857</v>
+      </c>
+      <c r="D31" t="s">
+        <v>858</v>
+      </c>
+      <c r="E31" t="s">
+        <v>818</v>
+      </c>
+      <c r="F31" t="s">
+        <v>819</v>
+      </c>
+      <c r="G31" t="s">
+        <v>820</v>
+      </c>
+      <c r="H31" t="s">
+        <v>821</v>
+      </c>
+      <c r="I31" t="s">
+        <v>822</v>
+      </c>
+      <c r="J31" t="s">
+        <v>823</v>
+      </c>
+      <c r="K31" t="s">
+        <v>824</v>
+      </c>
+      <c r="L31" t="s">
+        <v>825</v>
+      </c>
+      <c r="M31" t="s">
+        <v>826</v>
+      </c>
+      <c r="N31" t="s">
+        <v>827</v>
+      </c>
+      <c r="O31" t="s">
+        <v>828</v>
+      </c>
+      <c r="P31" t="s">
+        <v>829</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>830</v>
+      </c>
+      <c r="R31" t="s">
+        <v>831</v>
+      </c>
+      <c r="S31" t="s">
+        <v>832</v>
+      </c>
+      <c r="T31" t="s">
+        <v>833</v>
+      </c>
+      <c r="U31" t="s">
+        <v>834</v>
+      </c>
+      <c r="V31" t="s">
+        <v>835</v>
+      </c>
+      <c r="W31" t="s">
+        <v>836</v>
+      </c>
+      <c r="X31" t="s">
+        <v>837</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>859</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>860</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>861</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>862</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>863</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>864</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>865</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>866</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>867</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>868</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>841</v>
+      </c>
+      <c r="B32" t="s">
+        <v>856</v>
+      </c>
+      <c r="C32" t="s">
+        <v>857</v>
+      </c>
+      <c r="D32" t="s">
+        <v>858</v>
+      </c>
+      <c r="E32" t="s">
+        <v>818</v>
+      </c>
+      <c r="F32" t="s">
+        <v>819</v>
+      </c>
+      <c r="G32" t="s">
+        <v>820</v>
+      </c>
+      <c r="H32" t="s">
+        <v>821</v>
+      </c>
+      <c r="I32" t="s">
+        <v>822</v>
+      </c>
+      <c r="J32" t="s">
+        <v>823</v>
+      </c>
+      <c r="K32" t="s">
+        <v>824</v>
+      </c>
+      <c r="L32" t="s">
+        <v>825</v>
+      </c>
+      <c r="M32" t="s">
+        <v>826</v>
+      </c>
+      <c r="N32" t="s">
+        <v>827</v>
+      </c>
+      <c r="O32" t="s">
+        <v>828</v>
+      </c>
+      <c r="P32" t="s">
+        <v>829</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>830</v>
+      </c>
+      <c r="R32" t="s">
+        <v>831</v>
+      </c>
+      <c r="S32" t="s">
+        <v>832</v>
+      </c>
+      <c r="T32" t="s">
+        <v>833</v>
+      </c>
+      <c r="U32" t="s">
+        <v>834</v>
+      </c>
+      <c r="V32" t="s">
+        <v>835</v>
+      </c>
+      <c r="W32" t="s">
+        <v>836</v>
+      </c>
+      <c r="X32" t="s">
+        <v>837</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>859</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>860</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>861</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>862</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>863</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>864</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>865</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>866</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>867</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>868</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="B33" t="s">
+        <v>856</v>
+      </c>
+      <c r="C33" t="s">
+        <v>857</v>
+      </c>
+      <c r="D33" t="s">
+        <v>858</v>
+      </c>
+      <c r="E33" t="s">
+        <v>818</v>
+      </c>
+      <c r="F33" t="s">
+        <v>819</v>
+      </c>
+      <c r="G33" t="s">
+        <v>820</v>
+      </c>
+      <c r="H33" t="s">
+        <v>821</v>
+      </c>
+      <c r="I33" t="s">
+        <v>822</v>
+      </c>
+      <c r="J33" t="s">
+        <v>823</v>
+      </c>
+      <c r="K33" t="s">
+        <v>824</v>
+      </c>
+      <c r="L33" t="s">
+        <v>825</v>
+      </c>
+      <c r="M33" t="s">
+        <v>826</v>
+      </c>
+      <c r="N33" t="s">
+        <v>829</v>
+      </c>
+      <c r="O33" t="s">
+        <v>830</v>
+      </c>
+      <c r="P33" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>832</v>
+      </c>
+      <c r="R33" t="s">
+        <v>833</v>
+      </c>
+      <c r="S33" t="s">
+        <v>834</v>
+      </c>
+      <c r="T33" t="s">
+        <v>835</v>
+      </c>
+      <c r="U33" t="s">
+        <v>836</v>
+      </c>
+      <c r="V33" t="s">
+        <v>837</v>
+      </c>
+      <c r="W33" t="s">
+        <v>859</v>
+      </c>
+      <c r="X33" t="s">
+        <v>860</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>861</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>862</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>863</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>864</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>865</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>866</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>867</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>868</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>